<commit_message>
Added a README sheet to  CMOs-proposal-spreadsheet.xlsx
 explaining that it is a helper for the CMOs proposal

 pointing to the CMOs proposal itself in case something is found this file in isolation

 and explaining that it is used to delineate which combinations are desirable
</commit_message>
<xml_diff>
--- a/CMOs-proposal-spreadsheet.xlsx
+++ b/CMOs-proposal-spreadsheet.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glew\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glew\Documents\GitHub\Ri5-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3D5D6DF-EC89-48C5-AEDD-50AF844CBA73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9995FA-7E1B-4004-84D4-581FC50E069C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="-19452" windowWidth="30936" windowHeight="18816" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5940" yWindow="-19452" windowWidth="30936" windowHeight="18816" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counting" sheetId="2" r:id="rId1"/>
     <sheet name="Original" sheetId="1" r:id="rId2"/>
+    <sheet name="README" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -322,7 +322,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="221">
   <si>
     <t>User Abstract</t>
   </si>
@@ -1086,6 +1086,30 @@
   </si>
   <si>
     <t>Shorter Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">README for CMOs-proposal-spreadsheet.xlsx
+This spreadsheet is written in support of a proposal for CMOs (Cash Management Operations, also Prefetches) for RISC-V.
+The actual proposal is AsciiDoc text from which HTML and PDF are generated. The AsciiDoc source files themselves live in a GitHub wiki, whereas this file CMOs-proposal-spreadsheet.xlsx live in the corresponding GitHub repo.
+See https://github.com/AndyGlew/Ri5-stuff/wiki/Ri5-CMOs-proposal
+and in particular https://github.com/AndyGlew/Ri5-stuff/wiki/generated-HTML-and-PDF-for-CMOs-proposal
+With the latter pointing you to the generated files
+HTML: https://htmlpreview.github.io/?https://github.com/AndyGlew/Ri5-stuff/blob/master/Ri5-CMOs-proposal.html
+and
+PDF: https://github.com/AndyGlew/Ri5-stuff/blob/master/Ri5-CMOs-proposal.pdf
+The pointers replicated here so that you can find them more easily.
+Of course, this is all versioned, and a copy online may not be the latest copy - although it is the latest copy online on GitHub at those locations.
+The CMOs proposal describes almost orthogonal concepts of
+CMO operations: CLEAN, FLUSH, etc
+What parts of the memory subsystem they apply to: I$, D$, L2$ ... NVRAM
+Other considerations, such as local/global, and security.
+These are not fully orthogonal, some combinations do not make sense.
+This spreadsheet helps to understand which combinations make sense.
+If I had my way I would express these as a fully orthogonal set of fields in a CSR... And simply say that certain combinations are not permitted.
+But since I am being forced to put them into the actual instruction encoding, I want to reduce the number, not provide many combinations that are impossible. 
+The exercises also useful, because if we were doing the smart thing and actually putting them into a CSR, it would help understand which combinations are not allowed.
+Note: RISC-V is strongly against data value dependent exceptions. So if we did put these into a CSR, we would not be able to do illegal value detections at the time of write. Instead, we would do illegal value detection at the time of use.
+</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" textRotation="45"/>
@@ -1835,6 +1859,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1850,47 +1916,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6211,14 +6238,14 @@
       <c r="W9" s="42"/>
       <c r="X9" s="42"/>
       <c r="Y9" s="42"/>
-      <c r="Z9" s="141"/>
-      <c r="AA9" s="142"/>
-      <c r="AB9" s="142"/>
-      <c r="AC9" s="142"/>
-      <c r="AD9" s="142"/>
-      <c r="AE9" s="142"/>
-      <c r="AF9" s="142"/>
-      <c r="AG9" s="143"/>
+      <c r="Z9" s="155"/>
+      <c r="AA9" s="156"/>
+      <c r="AB9" s="156"/>
+      <c r="AC9" s="156"/>
+      <c r="AD9" s="156"/>
+      <c r="AE9" s="156"/>
+      <c r="AF9" s="156"/>
+      <c r="AG9" s="157"/>
       <c r="AH9" s="42"/>
       <c r="AI9" s="43"/>
       <c r="AJ9" s="42"/>
@@ -7818,158 +7845,158 @@
       <c r="BS21" s="38"/>
       <c r="BT21" s="37"/>
     </row>
-    <row r="22" spans="2:72" s="159" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="146"/>
-      <c r="C22" s="147" t="s">
+    <row r="22" spans="2:72" s="154" customFormat="1" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="141"/>
+      <c r="C22" s="142" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="147"/>
-      <c r="E22" s="148"/>
-      <c r="F22" s="148"/>
-      <c r="G22" s="149"/>
-      <c r="H22" s="150" t="s">
+      <c r="D22" s="142"/>
+      <c r="E22" s="143"/>
+      <c r="F22" s="143"/>
+      <c r="G22" s="144"/>
+      <c r="H22" s="145" t="s">
         <v>147</v>
       </c>
-      <c r="I22" s="151" t="s">
+      <c r="I22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="J22" s="152" t="s">
+      <c r="J22" s="147" t="s">
         <v>125</v>
       </c>
-      <c r="K22" s="151" t="s">
+      <c r="K22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="L22" s="152" t="s">
+      <c r="L22" s="147" t="s">
         <v>76</v>
       </c>
-      <c r="M22" s="152" t="s">
+      <c r="M22" s="147" t="s">
         <v>38</v>
       </c>
-      <c r="N22" s="151" t="s">
+      <c r="N22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="O22" s="152" t="s">
+      <c r="O22" s="147" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="152" t="s">
+      <c r="P22" s="147" t="s">
         <v>137</v>
       </c>
-      <c r="Q22" s="152" t="s">
+      <c r="Q22" s="147" t="s">
         <v>138</v>
       </c>
-      <c r="R22" s="152" t="s">
+      <c r="R22" s="147" t="s">
         <v>139</v>
       </c>
-      <c r="S22" s="152" t="s">
+      <c r="S22" s="147" t="s">
         <v>140</v>
       </c>
-      <c r="T22" s="151" t="s">
+      <c r="T22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="U22" s="152" t="s">
+      <c r="U22" s="147" t="s">
         <v>24</v>
       </c>
-      <c r="V22" s="151" t="s">
+      <c r="V22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="W22" s="152" t="s">
+      <c r="W22" s="147" t="s">
         <v>61</v>
       </c>
-      <c r="X22" s="152" t="s">
+      <c r="X22" s="147" t="s">
         <v>70</v>
       </c>
-      <c r="Y22" s="151" t="s">
+      <c r="Y22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="Z22" s="153" t="s">
+      <c r="Z22" s="148" t="s">
         <v>142</v>
       </c>
-      <c r="AA22" s="152" t="s">
+      <c r="AA22" s="147" t="s">
         <v>12</v>
       </c>
-      <c r="AB22" s="152" t="s">
+      <c r="AB22" s="147" t="s">
         <v>17</v>
       </c>
-      <c r="AC22" s="152" t="s">
+      <c r="AC22" s="147" t="s">
         <v>57</v>
       </c>
-      <c r="AD22" s="152" t="s">
+      <c r="AD22" s="147" t="s">
         <v>102</v>
       </c>
-      <c r="AE22" s="152" t="s">
+      <c r="AE22" s="147" t="s">
         <v>56</v>
       </c>
-      <c r="AF22" s="152" t="s">
+      <c r="AF22" s="147" t="s">
         <v>65</v>
       </c>
-      <c r="AG22" s="152" t="s">
+      <c r="AG22" s="147" t="s">
         <v>66</v>
       </c>
-      <c r="AH22" s="151" t="s">
+      <c r="AH22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="AI22" s="154" t="s">
+      <c r="AI22" s="149" t="s">
         <v>95</v>
       </c>
-      <c r="AJ22" s="152"/>
-      <c r="AK22" s="151" t="s">
+      <c r="AJ22" s="147"/>
+      <c r="AK22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="AL22" s="153" t="s">
+      <c r="AL22" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="AM22" s="153"/>
-      <c r="AN22" s="153"/>
-      <c r="AO22" s="153"/>
-      <c r="AP22" s="153"/>
-      <c r="AQ22" s="153"/>
-      <c r="AR22" s="155"/>
-      <c r="AS22" s="153"/>
-      <c r="AT22" s="153"/>
-      <c r="AU22" s="153"/>
-      <c r="AV22" s="153"/>
-      <c r="AW22" s="152"/>
-      <c r="AX22" s="156" t="s">
+      <c r="AM22" s="148"/>
+      <c r="AN22" s="148"/>
+      <c r="AO22" s="148"/>
+      <c r="AP22" s="148"/>
+      <c r="AQ22" s="148"/>
+      <c r="AR22" s="150"/>
+      <c r="AS22" s="148"/>
+      <c r="AT22" s="148"/>
+      <c r="AU22" s="148"/>
+      <c r="AV22" s="148"/>
+      <c r="AW22" s="147"/>
+      <c r="AX22" s="151" t="s">
         <v>197</v>
       </c>
-      <c r="AY22" s="152"/>
-      <c r="AZ22" s="157" t="s">
+      <c r="AY22" s="147"/>
+      <c r="AZ22" s="152" t="s">
         <v>198</v>
       </c>
-      <c r="BA22" s="152"/>
-      <c r="BB22" s="156" t="s">
+      <c r="BA22" s="147"/>
+      <c r="BB22" s="151" t="s">
         <v>199</v>
       </c>
-      <c r="BC22" s="152"/>
-      <c r="BD22" s="156" t="s">
+      <c r="BC22" s="147"/>
+      <c r="BD22" s="151" t="s">
         <v>201</v>
       </c>
-      <c r="BE22" s="152"/>
-      <c r="BF22" s="156" t="s">
+      <c r="BE22" s="147"/>
+      <c r="BF22" s="151" t="s">
         <v>202</v>
       </c>
-      <c r="BG22" s="152"/>
-      <c r="BH22" s="156" t="s">
+      <c r="BG22" s="147"/>
+      <c r="BH22" s="151" t="s">
         <v>16</v>
       </c>
-      <c r="BI22" s="152"/>
-      <c r="BJ22" s="156"/>
-      <c r="BK22" s="152"/>
-      <c r="BL22" s="156" t="s">
+      <c r="BI22" s="147"/>
+      <c r="BJ22" s="151"/>
+      <c r="BK22" s="147"/>
+      <c r="BL22" s="151" t="s">
         <v>200</v>
       </c>
-      <c r="BM22" s="152"/>
-      <c r="BN22" s="156" t="s">
+      <c r="BM22" s="147"/>
+      <c r="BN22" s="151" t="s">
         <v>200</v>
       </c>
-      <c r="BO22" s="152"/>
-      <c r="BP22" s="151" t="s">
+      <c r="BO22" s="147"/>
+      <c r="BP22" s="146" t="s">
         <v>1</v>
       </c>
-      <c r="BQ22" s="152"/>
-      <c r="BR22" s="152"/>
-      <c r="BS22" s="148"/>
-      <c r="BT22" s="158"/>
+      <c r="BQ22" s="147"/>
+      <c r="BR22" s="147"/>
+      <c r="BS22" s="143"/>
+      <c r="BT22" s="153"/>
     </row>
     <row r="23" spans="2:72" ht="43" x14ac:dyDescent="0.5">
       <c r="B23" s="37"/>
@@ -8999,7 +9026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:AZ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="5" ySplit="6" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="D4" sqref="D4"/>
@@ -9361,14 +9388,14 @@
       <c r="U9" s="42"/>
       <c r="V9" s="42"/>
       <c r="W9" s="42"/>
-      <c r="X9" s="141"/>
-      <c r="Y9" s="142"/>
-      <c r="Z9" s="142"/>
-      <c r="AA9" s="142"/>
-      <c r="AB9" s="142"/>
-      <c r="AC9" s="142"/>
-      <c r="AD9" s="142"/>
-      <c r="AE9" s="143"/>
+      <c r="X9" s="155"/>
+      <c r="Y9" s="156"/>
+      <c r="Z9" s="156"/>
+      <c r="AA9" s="156"/>
+      <c r="AB9" s="156"/>
+      <c r="AC9" s="156"/>
+      <c r="AD9" s="156"/>
+      <c r="AE9" s="157"/>
       <c r="AF9" s="42"/>
       <c r="AG9" s="43"/>
       <c r="AH9" s="42"/>
@@ -12005,7 +12032,7 @@
       <c r="AV42" s="26"/>
       <c r="AW42" s="26"/>
       <c r="AX42" s="72"/>
-      <c r="AY42" s="144" t="s">
+      <c r="AY42" s="158" t="s">
         <v>36</v>
       </c>
       <c r="AZ42" s="12"/>
@@ -12099,7 +12126,7 @@
       <c r="AV43" s="26"/>
       <c r="AW43" s="26"/>
       <c r="AX43" s="73"/>
-      <c r="AY43" s="145"/>
+      <c r="AY43" s="159"/>
       <c r="AZ43" s="12"/>
     </row>
     <row r="44" spans="2:52" ht="28.7" outlineLevel="1" x14ac:dyDescent="0.5">
@@ -14891,4 +14918,691 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24014F00-F21C-495E-AD41-ECE83726E7C1}">
+  <dimension ref="A1:P37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A1" s="160" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="160"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A2" s="160"/>
+      <c r="B2" s="160"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="160"/>
+      <c r="M2" s="160"/>
+      <c r="N2" s="160"/>
+      <c r="O2" s="160"/>
+      <c r="P2" s="160"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A3" s="160"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="160"/>
+      <c r="K3" s="160"/>
+      <c r="L3" s="160"/>
+      <c r="M3" s="160"/>
+      <c r="N3" s="160"/>
+      <c r="O3" s="160"/>
+      <c r="P3" s="160"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A4" s="160"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
+      <c r="H4" s="160"/>
+      <c r="I4" s="160"/>
+      <c r="J4" s="160"/>
+      <c r="K4" s="160"/>
+      <c r="L4" s="160"/>
+      <c r="M4" s="160"/>
+      <c r="N4" s="160"/>
+      <c r="O4" s="160"/>
+      <c r="P4" s="160"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A5" s="160"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="160"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="160"/>
+      <c r="K5" s="160"/>
+      <c r="L5" s="160"/>
+      <c r="M5" s="160"/>
+      <c r="N5" s="160"/>
+      <c r="O5" s="160"/>
+      <c r="P5" s="160"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A6" s="160"/>
+      <c r="B6" s="160"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
+      <c r="F6" s="160"/>
+      <c r="G6" s="160"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="160"/>
+      <c r="K6" s="160"/>
+      <c r="L6" s="160"/>
+      <c r="M6" s="160"/>
+      <c r="N6" s="160"/>
+      <c r="O6" s="160"/>
+      <c r="P6" s="160"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A7" s="160"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="160"/>
+      <c r="E7" s="160"/>
+      <c r="F7" s="160"/>
+      <c r="G7" s="160"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="160"/>
+      <c r="L7" s="160"/>
+      <c r="M7" s="160"/>
+      <c r="N7" s="160"/>
+      <c r="O7" s="160"/>
+      <c r="P7" s="160"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A8" s="160"/>
+      <c r="B8" s="160"/>
+      <c r="C8" s="160"/>
+      <c r="D8" s="160"/>
+      <c r="E8" s="160"/>
+      <c r="F8" s="160"/>
+      <c r="G8" s="160"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="160"/>
+      <c r="K8" s="160"/>
+      <c r="L8" s="160"/>
+      <c r="M8" s="160"/>
+      <c r="N8" s="160"/>
+      <c r="O8" s="160"/>
+      <c r="P8" s="160"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A9" s="160"/>
+      <c r="B9" s="160"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="160"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="160"/>
+      <c r="K9" s="160"/>
+      <c r="L9" s="160"/>
+      <c r="M9" s="160"/>
+      <c r="N9" s="160"/>
+      <c r="O9" s="160"/>
+      <c r="P9" s="160"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A10" s="160"/>
+      <c r="B10" s="160"/>
+      <c r="C10" s="160"/>
+      <c r="D10" s="160"/>
+      <c r="E10" s="160"/>
+      <c r="F10" s="160"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="160"/>
+      <c r="K10" s="160"/>
+      <c r="L10" s="160"/>
+      <c r="M10" s="160"/>
+      <c r="N10" s="160"/>
+      <c r="O10" s="160"/>
+      <c r="P10" s="160"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A11" s="160"/>
+      <c r="B11" s="160"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="160"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="160"/>
+      <c r="G11" s="160"/>
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="160"/>
+      <c r="K11" s="160"/>
+      <c r="L11" s="160"/>
+      <c r="M11" s="160"/>
+      <c r="N11" s="160"/>
+      <c r="O11" s="160"/>
+      <c r="P11" s="160"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A12" s="160"/>
+      <c r="B12" s="160"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="160"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="160"/>
+      <c r="G12" s="160"/>
+      <c r="H12" s="160"/>
+      <c r="I12" s="160"/>
+      <c r="J12" s="160"/>
+      <c r="K12" s="160"/>
+      <c r="L12" s="160"/>
+      <c r="M12" s="160"/>
+      <c r="N12" s="160"/>
+      <c r="O12" s="160"/>
+      <c r="P12" s="160"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A13" s="160"/>
+      <c r="B13" s="160"/>
+      <c r="C13" s="160"/>
+      <c r="D13" s="160"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
+      <c r="L13" s="160"/>
+      <c r="M13" s="160"/>
+      <c r="N13" s="160"/>
+      <c r="O13" s="160"/>
+      <c r="P13" s="160"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A14" s="160"/>
+      <c r="B14" s="160"/>
+      <c r="C14" s="160"/>
+      <c r="D14" s="160"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
+      <c r="L14" s="160"/>
+      <c r="M14" s="160"/>
+      <c r="N14" s="160"/>
+      <c r="O14" s="160"/>
+      <c r="P14" s="160"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A15" s="160"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
+      <c r="L15" s="160"/>
+      <c r="M15" s="160"/>
+      <c r="N15" s="160"/>
+      <c r="O15" s="160"/>
+      <c r="P15" s="160"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A16" s="160"/>
+      <c r="B16" s="160"/>
+      <c r="C16" s="160"/>
+      <c r="D16" s="160"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
+      <c r="L16" s="160"/>
+      <c r="M16" s="160"/>
+      <c r="N16" s="160"/>
+      <c r="O16" s="160"/>
+      <c r="P16" s="160"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A17" s="160"/>
+      <c r="B17" s="160"/>
+      <c r="C17" s="160"/>
+      <c r="D17" s="160"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
+      <c r="L17" s="160"/>
+      <c r="M17" s="160"/>
+      <c r="N17" s="160"/>
+      <c r="O17" s="160"/>
+      <c r="P17" s="160"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A18" s="160"/>
+      <c r="B18" s="160"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="160"/>
+      <c r="E18" s="160"/>
+      <c r="F18" s="160"/>
+      <c r="G18" s="160"/>
+      <c r="H18" s="160"/>
+      <c r="I18" s="160"/>
+      <c r="J18" s="160"/>
+      <c r="K18" s="160"/>
+      <c r="L18" s="160"/>
+      <c r="M18" s="160"/>
+      <c r="N18" s="160"/>
+      <c r="O18" s="160"/>
+      <c r="P18" s="160"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A19" s="160"/>
+      <c r="B19" s="160"/>
+      <c r="C19" s="160"/>
+      <c r="D19" s="160"/>
+      <c r="E19" s="160"/>
+      <c r="F19" s="160"/>
+      <c r="G19" s="160"/>
+      <c r="H19" s="160"/>
+      <c r="I19" s="160"/>
+      <c r="J19" s="160"/>
+      <c r="K19" s="160"/>
+      <c r="L19" s="160"/>
+      <c r="M19" s="160"/>
+      <c r="N19" s="160"/>
+      <c r="O19" s="160"/>
+      <c r="P19" s="160"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A20" s="160"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+      <c r="J20" s="160"/>
+      <c r="K20" s="160"/>
+      <c r="L20" s="160"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="160"/>
+      <c r="P20" s="160"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A21" s="160"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="160"/>
+      <c r="D21" s="160"/>
+      <c r="E21" s="160"/>
+      <c r="F21" s="160"/>
+      <c r="G21" s="160"/>
+      <c r="H21" s="160"/>
+      <c r="I21" s="160"/>
+      <c r="J21" s="160"/>
+      <c r="K21" s="160"/>
+      <c r="L21" s="160"/>
+      <c r="M21" s="160"/>
+      <c r="N21" s="160"/>
+      <c r="O21" s="160"/>
+      <c r="P21" s="160"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A22" s="160"/>
+      <c r="B22" s="160"/>
+      <c r="C22" s="160"/>
+      <c r="D22" s="160"/>
+      <c r="E22" s="160"/>
+      <c r="F22" s="160"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="160"/>
+      <c r="I22" s="160"/>
+      <c r="J22" s="160"/>
+      <c r="K22" s="160"/>
+      <c r="L22" s="160"/>
+      <c r="M22" s="160"/>
+      <c r="N22" s="160"/>
+      <c r="O22" s="160"/>
+      <c r="P22" s="160"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A23" s="160"/>
+      <c r="B23" s="160"/>
+      <c r="C23" s="160"/>
+      <c r="D23" s="160"/>
+      <c r="E23" s="160"/>
+      <c r="F23" s="160"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+      <c r="J23" s="160"/>
+      <c r="K23" s="160"/>
+      <c r="L23" s="160"/>
+      <c r="M23" s="160"/>
+      <c r="N23" s="160"/>
+      <c r="O23" s="160"/>
+      <c r="P23" s="160"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A24" s="160"/>
+      <c r="B24" s="160"/>
+      <c r="C24" s="160"/>
+      <c r="D24" s="160"/>
+      <c r="E24" s="160"/>
+      <c r="F24" s="160"/>
+      <c r="G24" s="160"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+      <c r="J24" s="160"/>
+      <c r="K24" s="160"/>
+      <c r="L24" s="160"/>
+      <c r="M24" s="160"/>
+      <c r="N24" s="160"/>
+      <c r="O24" s="160"/>
+      <c r="P24" s="160"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A25" s="160"/>
+      <c r="B25" s="160"/>
+      <c r="C25" s="160"/>
+      <c r="D25" s="160"/>
+      <c r="E25" s="160"/>
+      <c r="F25" s="160"/>
+      <c r="G25" s="160"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="160"/>
+      <c r="J25" s="160"/>
+      <c r="K25" s="160"/>
+      <c r="L25" s="160"/>
+      <c r="M25" s="160"/>
+      <c r="N25" s="160"/>
+      <c r="O25" s="160"/>
+      <c r="P25" s="160"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A26" s="160"/>
+      <c r="B26" s="160"/>
+      <c r="C26" s="160"/>
+      <c r="D26" s="160"/>
+      <c r="E26" s="160"/>
+      <c r="F26" s="160"/>
+      <c r="G26" s="160"/>
+      <c r="H26" s="160"/>
+      <c r="I26" s="160"/>
+      <c r="J26" s="160"/>
+      <c r="K26" s="160"/>
+      <c r="L26" s="160"/>
+      <c r="M26" s="160"/>
+      <c r="N26" s="160"/>
+      <c r="O26" s="160"/>
+      <c r="P26" s="160"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A27" s="160"/>
+      <c r="B27" s="160"/>
+      <c r="C27" s="160"/>
+      <c r="D27" s="160"/>
+      <c r="E27" s="160"/>
+      <c r="F27" s="160"/>
+      <c r="G27" s="160"/>
+      <c r="H27" s="160"/>
+      <c r="I27" s="160"/>
+      <c r="J27" s="160"/>
+      <c r="K27" s="160"/>
+      <c r="L27" s="160"/>
+      <c r="M27" s="160"/>
+      <c r="N27" s="160"/>
+      <c r="O27" s="160"/>
+      <c r="P27" s="160"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A28" s="160"/>
+      <c r="B28" s="160"/>
+      <c r="C28" s="160"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="160"/>
+      <c r="F28" s="160"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="160"/>
+      <c r="I28" s="160"/>
+      <c r="J28" s="160"/>
+      <c r="K28" s="160"/>
+      <c r="L28" s="160"/>
+      <c r="M28" s="160"/>
+      <c r="N28" s="160"/>
+      <c r="O28" s="160"/>
+      <c r="P28" s="160"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A29" s="160"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="160"/>
+      <c r="D29" s="160"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="160"/>
+      <c r="I29" s="160"/>
+      <c r="J29" s="160"/>
+      <c r="K29" s="160"/>
+      <c r="L29" s="160"/>
+      <c r="M29" s="160"/>
+      <c r="N29" s="160"/>
+      <c r="O29" s="160"/>
+      <c r="P29" s="160"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A30" s="160"/>
+      <c r="B30" s="160"/>
+      <c r="C30" s="160"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="160"/>
+      <c r="F30" s="160"/>
+      <c r="G30" s="160"/>
+      <c r="H30" s="160"/>
+      <c r="I30" s="160"/>
+      <c r="J30" s="160"/>
+      <c r="K30" s="160"/>
+      <c r="L30" s="160"/>
+      <c r="M30" s="160"/>
+      <c r="N30" s="160"/>
+      <c r="O30" s="160"/>
+      <c r="P30" s="160"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A31" s="160"/>
+      <c r="B31" s="160"/>
+      <c r="C31" s="160"/>
+      <c r="D31" s="160"/>
+      <c r="E31" s="160"/>
+      <c r="F31" s="160"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="160"/>
+      <c r="I31" s="160"/>
+      <c r="J31" s="160"/>
+      <c r="K31" s="160"/>
+      <c r="L31" s="160"/>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="160"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A32" s="160"/>
+      <c r="B32" s="160"/>
+      <c r="C32" s="160"/>
+      <c r="D32" s="160"/>
+      <c r="E32" s="160"/>
+      <c r="F32" s="160"/>
+      <c r="G32" s="160"/>
+      <c r="H32" s="160"/>
+      <c r="I32" s="160"/>
+      <c r="J32" s="160"/>
+      <c r="K32" s="160"/>
+      <c r="L32" s="160"/>
+      <c r="M32" s="160"/>
+      <c r="N32" s="160"/>
+      <c r="O32" s="160"/>
+      <c r="P32" s="160"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A33" s="160"/>
+      <c r="B33" s="160"/>
+      <c r="C33" s="160"/>
+      <c r="D33" s="160"/>
+      <c r="E33" s="160"/>
+      <c r="F33" s="160"/>
+      <c r="G33" s="160"/>
+      <c r="H33" s="160"/>
+      <c r="I33" s="160"/>
+      <c r="J33" s="160"/>
+      <c r="K33" s="160"/>
+      <c r="L33" s="160"/>
+      <c r="M33" s="160"/>
+      <c r="N33" s="160"/>
+      <c r="O33" s="160"/>
+      <c r="P33" s="160"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A34" s="160"/>
+      <c r="B34" s="160"/>
+      <c r="C34" s="160"/>
+      <c r="D34" s="160"/>
+      <c r="E34" s="160"/>
+      <c r="F34" s="160"/>
+      <c r="G34" s="160"/>
+      <c r="H34" s="160"/>
+      <c r="I34" s="160"/>
+      <c r="J34" s="160"/>
+      <c r="K34" s="160"/>
+      <c r="L34" s="160"/>
+      <c r="M34" s="160"/>
+      <c r="N34" s="160"/>
+      <c r="O34" s="160"/>
+      <c r="P34" s="160"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A35" s="160"/>
+      <c r="B35" s="160"/>
+      <c r="C35" s="160"/>
+      <c r="D35" s="160"/>
+      <c r="E35" s="160"/>
+      <c r="F35" s="160"/>
+      <c r="G35" s="160"/>
+      <c r="H35" s="160"/>
+      <c r="I35" s="160"/>
+      <c r="J35" s="160"/>
+      <c r="K35" s="160"/>
+      <c r="L35" s="160"/>
+      <c r="M35" s="160"/>
+      <c r="N35" s="160"/>
+      <c r="O35" s="160"/>
+      <c r="P35" s="160"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A36" s="160"/>
+      <c r="B36" s="160"/>
+      <c r="C36" s="160"/>
+      <c r="D36" s="160"/>
+      <c r="E36" s="160"/>
+      <c r="F36" s="160"/>
+      <c r="G36" s="160"/>
+      <c r="H36" s="160"/>
+      <c r="I36" s="160"/>
+      <c r="J36" s="160"/>
+      <c r="K36" s="160"/>
+      <c r="L36" s="160"/>
+      <c r="M36" s="160"/>
+      <c r="N36" s="160"/>
+      <c r="O36" s="160"/>
+      <c r="P36" s="160"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.5">
+      <c r="A37" s="160"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="160"/>
+      <c r="D37" s="160"/>
+      <c r="E37" s="160"/>
+      <c r="F37" s="160"/>
+      <c r="G37" s="160"/>
+      <c r="H37" s="160"/>
+      <c r="I37" s="160"/>
+      <c r="J37" s="160"/>
+      <c r="K37" s="160"/>
+      <c r="L37" s="160"/>
+      <c r="M37" s="160"/>
+      <c r="N37" s="160"/>
+      <c r="O37" s="160"/>
+      <c r="P37" s="160"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>